<commit_message>
Practice with Excel and Data Tables
</commit_message>
<xml_diff>
--- a/UiPath Beginners Course/FirstRobot/Excel and Data Tables/Orders.xlsx
+++ b/UiPath Beginners Course/FirstRobot/Excel and Data Tables/Orders.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49287199858e515f/RPAnders/Anders Jensen/Projects/20200202 UiPath Beginners Vs2/Course/Files/Excel and Data Tables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitRepo\UiPathLearning\UiPath Beginners Course\FirstRobot\Excel and Data Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="38" documentId="11_F25DC773A252ABDACC1048C4E99D741A5ADE58EE" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{245B21AA-5D44-4A43-A54A-707DD19453ED}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ED3CA30-495B-404D-8EAC-309DAC9889C7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2310" yWindow="1875" windowWidth="20070" windowHeight="13905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39315" yWindow="915" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Orders" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>OrderID</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>Peaches</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -95,7 +98,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -376,12 +379,12 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -401,7 +404,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -414,9 +417,14 @@
       <c r="D2" s="1">
         <v>2</v>
       </c>
-      <c r="E2" s="1"/>
+      <c r="E2" s="1">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -429,9 +437,11 @@
       <c r="D3" s="1">
         <v>1</v>
       </c>
-      <c r="E3" s="1"/>
+      <c r="E3" s="1">
+        <v>6</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -444,9 +454,11 @@
       <c r="D4" s="1">
         <v>1</v>
       </c>
-      <c r="E4" s="1"/>
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -459,7 +471,12 @@
       <c r="D5" s="1">
         <v>3</v>
       </c>
-      <c r="E5" s="1"/>
+      <c r="E5" s="1">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>